<commit_message>
continuing work on exercise1
</commit_message>
<xml_diff>
--- a/ASM109_2021_data/AE4ASM109(dimensions).xlsx
+++ b/ASM109_2021_data/AE4ASM109(dimensions).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mortezamoradi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d606a05df2b91673/Dokument/GitHub/DACS/ASM109_2021_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_26C445E52044405B7AA6112F477C78261CAB772F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F27FE6DA-B4EF-4293-9ADE-96A7CBD1022E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UD" sheetId="1" r:id="rId1"/>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -248,15 +249,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -265,7 +263,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -280,19 +287,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -574,104 +572,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="11.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="4"/>
+    <col min="2" max="2" width="9.109375" style="2"/>
+    <col min="3" max="3" width="9.109375" style="3"/>
+    <col min="4" max="4" width="9.109375" style="2"/>
+    <col min="5" max="5" width="9.109375" style="1"/>
+    <col min="6" max="6" width="9.109375" style="3"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="8" width="9.109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="1"/>
+    <col min="11" max="11" width="11.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>250.17</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>250.19</v>
       </c>
       <c r="D3" s="2">
         <v>14.98</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>14.99</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>14.99</v>
       </c>
       <c r="G3" s="1">
@@ -693,23 +691,23 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>250.16</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>250.13</v>
       </c>
       <c r="D4" s="2">
         <v>15.14</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>15.12</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>15.15</v>
       </c>
       <c r="G4" s="1">
@@ -731,23 +729,23 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>250.15</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>250.13</v>
       </c>
       <c r="D5" s="2">
         <v>15.2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>15.17</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>15.16</v>
       </c>
       <c r="G5" s="1">
@@ -769,23 +767,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>250.14</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>250.15</v>
       </c>
       <c r="D6" s="2">
         <v>15.12</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>15.11</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>15.1</v>
       </c>
       <c r="G6" s="1">
@@ -807,23 +805,23 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>250.15</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>250.15</v>
       </c>
       <c r="D7" s="2">
         <v>15.09</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>15.09</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>15.09</v>
       </c>
       <c r="G7" s="1">
@@ -845,23 +843,23 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>250.16</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>250.16</v>
       </c>
       <c r="D8" s="2">
         <v>15.12</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>15.07</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>15.1</v>
       </c>
       <c r="G8" s="1">
@@ -883,23 +881,23 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>250.18</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>250.16</v>
       </c>
       <c r="D9" s="2">
         <v>15.16</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>15.12</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>15.14</v>
       </c>
       <c r="G9" s="1">
@@ -921,23 +919,23 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>250.15</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>250.13</v>
       </c>
       <c r="D10" s="2">
         <v>15.16</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>15.13</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>15.15</v>
       </c>
       <c r="G10" s="1">
@@ -959,23 +957,23 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>250.13</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>250.11</v>
       </c>
       <c r="D11" s="2">
         <v>15.08</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>15.07</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>15.09</v>
       </c>
       <c r="G11" s="1">
@@ -997,23 +995,23 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>250.11</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>250.11</v>
       </c>
       <c r="D12" s="2">
         <v>15.16</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <v>15.14</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>15.17</v>
       </c>
       <c r="G12" s="1">
@@ -1035,23 +1033,23 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>250.11</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>250.13</v>
       </c>
       <c r="D13" s="2">
         <v>15.04</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="1">
         <v>15.05</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>15.09</v>
       </c>
       <c r="G13" s="1">
@@ -1073,23 +1071,23 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>250.16</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>250.17</v>
       </c>
       <c r="D14" s="2">
         <v>15.11</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="1">
         <v>15.1</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>15.16</v>
       </c>
       <c r="G14" s="1">
@@ -1111,23 +1109,23 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>250.17</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>250.15</v>
       </c>
       <c r="D15" s="2">
         <v>15.18</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="1">
         <v>15.1</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>15.15</v>
       </c>
       <c r="G15" s="1">
@@ -1149,23 +1147,23 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>250.15</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>250.11</v>
       </c>
       <c r="D16" s="2">
         <v>15.17</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="1">
         <v>15.12</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>15.15</v>
       </c>
       <c r="G16" s="1">
@@ -1187,23 +1185,23 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>250.11</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>250.11</v>
       </c>
       <c r="D17" s="2">
         <v>15.08</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="1">
         <v>15.07</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>15.1</v>
       </c>
       <c r="G17" s="1">
@@ -1225,23 +1223,23 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>250.1</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>250.1</v>
       </c>
       <c r="D18" s="2">
         <v>15.18</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="1">
         <v>15.12</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>15.4</v>
       </c>
       <c r="G18" s="1">
@@ -1263,23 +1261,23 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>250.09</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>250.08</v>
       </c>
       <c r="D19" s="2">
         <v>15.18</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="1">
         <v>15.11</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>15.36</v>
       </c>
       <c r="G19" s="1">
@@ -1314,104 +1312,104 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="11.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="4"/>
+    <col min="2" max="2" width="9.109375" style="2"/>
+    <col min="3" max="3" width="9.109375" style="3"/>
+    <col min="4" max="4" width="9.109375" style="2"/>
+    <col min="5" max="5" width="9.109375" style="1"/>
+    <col min="6" max="6" width="9.109375" style="3"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="8" width="9.109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="1"/>
+    <col min="11" max="11" width="11.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>175.12</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>175.11</v>
       </c>
       <c r="D3" s="2">
         <v>25.05</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>25.07</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>25.09</v>
       </c>
       <c r="G3" s="1">
@@ -1433,23 +1431,23 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>175.1</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>175.09</v>
       </c>
       <c r="D4" s="2">
         <v>24.99</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>24.97</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>24.92</v>
       </c>
       <c r="G4" s="1">
@@ -1471,23 +1469,23 @@
         <v>2.14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>175.12</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>175.11</v>
       </c>
       <c r="D5" s="2">
         <v>25.04</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>25.08</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>25.07</v>
       </c>
       <c r="G5" s="1">
@@ -1509,23 +1507,23 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>175.1</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>175.1</v>
       </c>
       <c r="D6" s="2">
         <v>25.04</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>25.05</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>25.05</v>
       </c>
       <c r="G6" s="1">
@@ -1547,23 +1545,23 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>175.1</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>175.1</v>
       </c>
       <c r="D7" s="2">
         <v>25.07</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>25.07</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>25.08</v>
       </c>
       <c r="G7" s="1">
@@ -1585,23 +1583,23 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>175.1</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>175.09</v>
       </c>
       <c r="D8" s="2">
         <v>25.02</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>25.05</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>25.03</v>
       </c>
       <c r="G8" s="1">
@@ -1623,23 +1621,23 @@
         <v>2.14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>175.08</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>175.08</v>
       </c>
       <c r="D9" s="2">
         <v>25.03</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>25.05</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>25.03</v>
       </c>
       <c r="G9" s="1">
@@ -1661,23 +1659,23 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>175.08</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>175.09</v>
       </c>
       <c r="D10" s="2">
         <v>25.06</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>25.06</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>25.06</v>
       </c>
       <c r="G10" s="1">
@@ -1699,23 +1697,23 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>175.07</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>175.06</v>
       </c>
       <c r="D11" s="2">
         <v>25</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>25.02</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>25.04</v>
       </c>
       <c r="G11" s="1">
@@ -1750,104 +1748,104 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="11.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="4"/>
+    <col min="2" max="2" width="9.109375" style="2"/>
+    <col min="3" max="3" width="9.109375" style="3"/>
+    <col min="4" max="4" width="9.109375" style="2"/>
+    <col min="5" max="5" width="9.109375" style="1"/>
+    <col min="6" max="6" width="9.109375" style="3"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="8" width="9.109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="1"/>
+    <col min="11" max="11" width="11.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>250.11</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>250.08</v>
       </c>
       <c r="D3" s="2">
         <v>25.03</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>25.03</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>25.05</v>
       </c>
       <c r="G3" s="1">
@@ -1869,23 +1867,23 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>250.09</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>250.08</v>
       </c>
       <c r="D4" s="2">
         <v>25.01</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>25.03</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>25.09</v>
       </c>
       <c r="G4" s="1">
@@ -1907,23 +1905,23 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>250.09</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>250.05</v>
       </c>
       <c r="D5" s="2">
         <v>24.95</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>25.02</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>25.09</v>
       </c>
       <c r="G5" s="1">
@@ -1945,23 +1943,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>250.06</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>250.06</v>
       </c>
       <c r="D6" s="2">
         <v>25.02</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>25.04</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>25.03</v>
       </c>
       <c r="G6" s="1">
@@ -1983,23 +1981,23 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>250.07</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>250.07</v>
       </c>
       <c r="D7" s="2">
         <v>25.02</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>25.07</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>25.16</v>
       </c>
       <c r="G7" s="1">
@@ -2021,23 +2019,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>250.07</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>250.07</v>
       </c>
       <c r="D8" s="2">
         <v>25.1</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>25.08</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>25.06</v>
       </c>
       <c r="G8" s="1">
@@ -2059,23 +2057,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>250.07</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>250.07</v>
       </c>
       <c r="D9" s="2">
         <v>25.05</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>25.05</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>25.05</v>
       </c>
       <c r="G9" s="1">
@@ -2097,23 +2095,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>250.06</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>250.06</v>
       </c>
       <c r="D10" s="2">
         <v>24.96</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>24.94</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>24.94</v>
       </c>
       <c r="G10" s="1">
@@ -2135,23 +2133,23 @@
         <v>2.06</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>250.06</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>250.07</v>
       </c>
       <c r="D11" s="2">
         <v>25.01</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>25.02</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>25.11</v>
       </c>
       <c r="G11" s="1">
@@ -2186,104 +2184,104 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="11.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="4"/>
+    <col min="2" max="2" width="9.109375" style="2"/>
+    <col min="3" max="3" width="9.109375" style="3"/>
+    <col min="4" max="4" width="9.109375" style="2"/>
+    <col min="5" max="5" width="9.109375" style="1"/>
+    <col min="6" max="6" width="9.109375" style="3"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="8" width="9.109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="1"/>
+    <col min="11" max="11" width="11.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>250.04</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>250.03</v>
       </c>
       <c r="D3" s="2">
         <v>25.05</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>25.06</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>25.07</v>
       </c>
       <c r="G3" s="1">
@@ -2305,23 +2303,23 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>250.04</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>250.05</v>
       </c>
       <c r="D4" s="2">
         <v>25.03</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>25.07</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>25.04</v>
       </c>
       <c r="G4" s="1">
@@ -2343,23 +2341,23 @@
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>250.04</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>250.05</v>
       </c>
       <c r="D5" s="2">
         <v>25.04</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>25.04</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>25.05</v>
       </c>
       <c r="G5" s="1">
@@ -2381,23 +2379,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>250.06</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>250.06</v>
       </c>
       <c r="D6" s="2">
         <v>25.06</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>25.06</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>25.07</v>
       </c>
       <c r="G6" s="1">
@@ -2419,23 +2417,23 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>250.07</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>250.07</v>
       </c>
       <c r="D7" s="2">
         <v>25.06</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>25.06</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>25.07</v>
       </c>
       <c r="G7" s="1">
@@ -2457,23 +2455,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>250.08</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>250.08</v>
       </c>
       <c r="D8" s="2">
         <v>25.07</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>25.05</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>25.08</v>
       </c>
       <c r="G8" s="1">
@@ -2495,23 +2493,23 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>250.08</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>250.08</v>
       </c>
       <c r="D9" s="2">
         <v>24.99</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>25</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>25.02</v>
       </c>
       <c r="G9" s="1">
@@ -2533,23 +2531,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>250.08</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>250.08</v>
       </c>
       <c r="D10" s="2">
         <v>25.08</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>25.08</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>25.16</v>
       </c>
       <c r="G10" s="1">
@@ -2571,23 +2569,23 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>250.11</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>250.12</v>
       </c>
       <c r="D11" s="2">
         <v>25.04</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>25.06</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>25.07</v>
       </c>
       <c r="G11" s="1">
@@ -2609,23 +2607,23 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>250.14</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>250.13</v>
       </c>
       <c r="D12" s="2">
         <v>25.07</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <v>25.07</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>25.06</v>
       </c>
       <c r="G12" s="1">

</xml_diff>